<commit_message>
dns stuff - aks
</commit_message>
<xml_diff>
--- a/azure_resources.xlsx
+++ b/azure_resources.xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/98c72bd1cd26f1f6/Works/github/config_mgtm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="11_0705C1882176DAB1EA7778E678CDFF5847934F84" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7F9E4BBB-A472-4920-87D5-0C6C27C960F2}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="11_611183940F4421B118B7A63DE90AE323A7916FFD" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{45381BEB-9508-442C-ACD4-E7EB4E2269C8}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
     <sheet name="Virtual Machines" sheetId="2" r:id="rId2"/>
-    <sheet name="App Services" sheetId="3" r:id="rId3"/>
+    <sheet name="AKS" sheetId="3" r:id="rId3"/>
+    <sheet name="App Services" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="62">
   <si>
     <t>Resource Group</t>
   </si>
@@ -57,9 +58,6 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>VM01.zjxrmllu3uqe1dsnmc1iyj14ng.dx.internal.cloudapp.net</t>
-  </si>
-  <si>
     <t>tagging</t>
   </si>
   <si>
@@ -103,6 +101,84 @@
   </si>
   <si>
     <t>custon-dns-temp.ooa40cmcdunezb0lgwfzv2nnxg.bx.internal.cloudapp.net</t>
+  </si>
+  <si>
+    <t>AKS Server</t>
+  </si>
+  <si>
+    <t>Namespace</t>
+  </si>
+  <si>
+    <t>Service</t>
+  </si>
+  <si>
+    <t>Service IP</t>
+  </si>
+  <si>
+    <t>DefaultResourceGroup-WUS2</t>
+  </si>
+  <si>
+    <t>aks-istio-system</t>
+  </si>
+  <si>
+    <t>istiod-asm-1-19</t>
+  </si>
+  <si>
+    <t>10.0.98.233</t>
+  </si>
+  <si>
+    <t>calico-system</t>
+  </si>
+  <si>
+    <t>calico-kube-controllers-metrics</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>calico-typha</t>
+  </si>
+  <si>
+    <t>10.0.203.206</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>kubernetes</t>
+  </si>
+  <si>
+    <t>10.0.0.1</t>
+  </si>
+  <si>
+    <t>gatekeeper-system</t>
+  </si>
+  <si>
+    <t>gatekeeper-webhook-service</t>
+  </si>
+  <si>
+    <t>10.0.220.234</t>
+  </si>
+  <si>
+    <t>kube-system</t>
+  </si>
+  <si>
+    <t>azure-policy-webhook-service</t>
+  </si>
+  <si>
+    <t>10.0.17.59</t>
+  </si>
+  <si>
+    <t>kube-dns</t>
+  </si>
+  <si>
+    <t>10.0.0.10</t>
+  </si>
+  <si>
+    <t>metrics-server</t>
+  </si>
+  <si>
+    <t>10.0.212.220</t>
   </si>
   <si>
     <t>App Services</t>
@@ -486,18 +562,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="15.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="63.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.1796875" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -536,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
@@ -547,19 +614,19 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>15</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
       </c>
       <c r="F3" t="s">
         <v>10</v>
@@ -570,48 +637,48 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
         <v>17</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>18</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>19</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>20</v>
-      </c>
-      <c r="E4" t="s">
-        <v>21</v>
       </c>
       <c r="F4" t="s">
         <v>10</v>
       </c>
       <c r="G4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
         <v>23</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>24</v>
-      </c>
-      <c r="C5" t="s">
-        <v>25</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F5" t="s">
         <v>10</v>
       </c>
       <c r="G5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -621,9 +688,160 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="25.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -632,41 +850,41 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="C1" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="D1" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="D3" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding aks gather ips
</commit_message>
<xml_diff>
--- a/azure_resources.xlsx
+++ b/azure_resources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/98c72bd1cd26f1f6/Works/github/config_mgtm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="11_611183940F4421B118B7A63DE90AE323A7916FFD" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{45381BEB-9508-442C-ACD4-E7EB4E2269C8}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="11_53A5E2960F4421B11827A897A56EC995A691E8B1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DF7953DA-D79E-4C49-9256-4908E10CBE4C}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="55">
   <si>
     <t>Resource Group</t>
   </si>
@@ -85,9 +85,6 @@
     <t>40.117.103.79</t>
   </si>
   <si>
-    <t>heider-temp-vm.ooa40cmcdunezb0lgwfzv2nnxg.bx.internal.cloudapp.net</t>
-  </si>
-  <si>
     <t>10.10.0.6, 10.10.0.7</t>
   </si>
   <si>
@@ -100,9 +97,6 @@
     <t>10.10.0.6</t>
   </si>
   <si>
-    <t>custon-dns-temp.ooa40cmcdunezb0lgwfzv2nnxg.bx.internal.cloudapp.net</t>
-  </si>
-  <si>
     <t>AKS Server</t>
   </si>
   <si>
@@ -115,16 +109,10 @@
     <t>Service IP</t>
   </si>
   <si>
-    <t>DefaultResourceGroup-WUS2</t>
-  </si>
-  <si>
-    <t>aks-istio-system</t>
-  </si>
-  <si>
-    <t>istiod-asm-1-19</t>
-  </si>
-  <si>
-    <t>10.0.98.233</t>
+    <t>MC_aks-heider_aks-heider-temp_eastus</t>
+  </si>
+  <si>
+    <t>aks-heider-temp</t>
   </si>
   <si>
     <t>calico-system</t>
@@ -139,7 +127,7 @@
     <t>calico-typha</t>
   </si>
   <si>
-    <t>10.0.203.206</t>
+    <t>10.0.226.138</t>
   </si>
   <si>
     <t>default</t>
@@ -151,24 +139,9 @@
     <t>10.0.0.1</t>
   </si>
   <si>
-    <t>gatekeeper-system</t>
-  </si>
-  <si>
-    <t>gatekeeper-webhook-service</t>
-  </si>
-  <si>
-    <t>10.0.220.234</t>
-  </si>
-  <si>
     <t>kube-system</t>
   </si>
   <si>
-    <t>azure-policy-webhook-service</t>
-  </si>
-  <si>
-    <t>10.0.17.59</t>
-  </si>
-  <si>
     <t>kube-dns</t>
   </si>
   <si>
@@ -178,7 +151,13 @@
     <t>metrics-server</t>
   </si>
   <si>
-    <t>10.0.212.220</t>
+    <t>10.0.2.10</t>
+  </si>
+  <si>
+    <t>MC_aks-heider_aks-test2-heider_westus</t>
+  </si>
+  <si>
+    <t>aks-test2-heider</t>
   </si>
   <si>
     <t>App Services</t>
@@ -649,36 +628,36 @@
         <v>19</v>
       </c>
       <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" t="s">
         <v>20</v>
-      </c>
-      <c r="F4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
         <v>22</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>23</v>
       </c>
-      <c r="C5" t="s">
-        <v>24</v>
-      </c>
       <c r="D5" t="s">
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="F5" t="s">
         <v>10</v>
       </c>
       <c r="G5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -688,17 +667,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.90625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.81640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.453125" bestFit="1" customWidth="1"/>
   </cols>
@@ -708,128 +685,186 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
         <v>26</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>27</v>
-      </c>
-      <c r="D1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" t="s">
         <v>30</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>31</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>32</v>
-      </c>
-      <c r="E2" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
         <v>30</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" t="s">
         <v>34</v>
-      </c>
-      <c r="D3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>28</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" t="s">
         <v>37</v>
-      </c>
-      <c r="E4" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>28</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
       </c>
       <c r="C5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" t="s">
         <v>39</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>40</v>
-      </c>
-      <c r="E5" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>28</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
       </c>
       <c r="C6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" t="s">
         <v>42</v>
-      </c>
-      <c r="D6" t="s">
-        <v>43</v>
-      </c>
-      <c r="E6" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" t="s">
         <v>30</v>
       </c>
-      <c r="C7" t="s">
-        <v>45</v>
-      </c>
       <c r="D7" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="E7" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" t="s">
         <v>30</v>
       </c>
-      <c r="C8" t="s">
-        <v>45</v>
-      </c>
       <c r="D8" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="E8" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>43</v>
+      </c>
+      <c r="B9" t="s">
+        <v>44</v>
       </c>
       <c r="C9" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="D9" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="E9" t="s">
-        <v>51</v>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -850,41 +885,41 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="D1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C2" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="D2" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C3" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="D3" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>